<commit_message>
Temporary solution for error handling on Repl expr on bad let variable
I had an error with push from previous commit; did not notice until trying to push. Updating T/L since then.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-25july2016.xlsx
+++ b/time-labor/week-of-25july2016.xlsx
@@ -57,6 +57,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -638,15 +639,15 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="7" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -968,13 +969,17 @@
       <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="0"/>
+      <c r="C17" s="19" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.583333333333333</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -1009,13 +1014,17 @@
       <c r="B19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="19" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D19" s="20" t="n">
+        <v>0.5625</v>
+      </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21" t="n">
         <f aca="false">IF((((D19-C19)+(F19-E19))*24)&gt;8,8,((D19-C19)+(F19-E19))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="21" t="n">
         <f aca="false">IF(((D19-C19)+(F19-E19))*24&gt;8,((D19-C19)+(F19-E19))*24-8,0)</f>
@@ -1035,7 +1044,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1079,7 +1088,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1095,7 +1104,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>140</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1109,6 +1118,7 @@
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="31"/>
@@ -1181,7 +1191,7 @@
     <mergeCell ref="F26:I26"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F16 C17:C19 E17:F17 D18:F19" type="time">
+    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F19" type="time">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>